<commit_message>
Calculated precision, recall and F1 score
</commit_message>
<xml_diff>
--- a/Strojer_Images/Only Aligned Dataset/evaluations/resultsIoU50OnlyAligned.xlsx
+++ b/Strojer_Images/Only Aligned Dataset/evaluations/resultsIoU50OnlyAligned.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
   <si>
     <t xml:space="preserve">File Name</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t xml:space="preserve">F1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Images with perfect score</t>
   </si>
 </sst>
 </file>
@@ -297,15 +300,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H41" activeCellId="0" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -1246,6 +1249,15 @@
       <c r="B57" s="0" t="n">
         <f aca="false">2*B55*B56/(B55+B56)</f>
         <v>0.895340985820392</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <f aca="false">COUNTIF(B2:B52,16)</f>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>